<commit_message>
b_sid: save for later added, add product change
</commit_message>
<xml_diff>
--- a/src/assets/docs/bulkProducts_all_ean_configured_example.xlsx
+++ b/src/assets/docs/bulkProducts_all_ean_configured_example.xlsx
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1106,7 @@
         <v>2400000011</v>
       </c>
       <c r="G2" s="5">
-        <v>2400000013</v>
+        <v>2400000018</v>
       </c>
       <c r="H2" t="s">
         <v>89</v>
@@ -1201,7 +1201,7 @@
         <v>2400000012</v>
       </c>
       <c r="G3" s="5">
-        <v>2400000014</v>
+        <v>240000001456</v>
       </c>
       <c r="H3" t="s">
         <v>102</v>

</xml_diff>